<commit_message>
[girish]taking the screenshot sending keys and implementing log4net
</commit_message>
<xml_diff>
--- a/AjioAutomation/ExcelData/TestData.xlsx
+++ b/AjioAutomation/ExcelData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20377"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E06FE3E-F527-4B1F-B221-A1033C113A20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E116904E-6FC9-4299-90A6-F4C96B8FCD2B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,29 +25,21 @@
     <t>email</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>girishvayugundla@gmail.com</t>
   </si>
   <si>
     <t>Girish@2505</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -82,12 +74,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -372,7 +364,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,19 +374,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>